<commit_message>
Plots Code, Images, and rearrange files
</commit_message>
<xml_diff>
--- a/dauer_pathway/LD/LD_between_paired_alleles_corr.xlsx
+++ b/dauer_pathway/LD/LD_between_paired_alleles_corr.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanmckeown/Documents/andersen_lab/data_exploration/del_explorers/dauer_pathway/LD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8711AE03-B52C-6640-B959-1C3B066CFAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9E18A7-3359-7E4C-BAF8-E4263A2105AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2240" yWindow="-20940" windowWidth="38400" windowHeight="21100"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32880" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LD_between_paired_alleles" sheetId="1" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -623,7 +623,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="19">
     <dxf>
       <border>
         <left style="thin">
@@ -911,26 +911,6 @@
           <color rgb="FF9C0006"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1251,11 +1231,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3035,7 +3015,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:X24">
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>